<commit_message>
MODIFY write names of material
</commit_message>
<xml_diff>
--- a/Documentation/Required Materials.xlsx
+++ b/Documentation/Required Materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jocor\Desktop\Projet de recherche\main\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32F5992-FBDA-459B-AF95-B19E1FE29C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE8AA99-EEE6-488D-910D-2ECC045C6AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
-  <si>
-    <t>GPS module</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Barometer</t>
   </si>
@@ -78,6 +75,27 @@
   </si>
   <si>
     <t>Raspberry Pi  Zero W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS module </t>
+  </si>
+  <si>
+    <t>(Whadda WPI430 Module GPS U-BLOX NEO-7M)</t>
+  </si>
+  <si>
+    <t>(DFRobot Gravity BMP388)</t>
+  </si>
+  <si>
+    <t>(Joy-it Module d'affichage Raspberry Pi® JT3.5TR)</t>
+  </si>
+  <si>
+    <t>amazon.fr</t>
+  </si>
+  <si>
+    <t>PiSugar Battery 1200 mAh</t>
+  </si>
+  <si>
+    <t>(PiSugar Pwnagotchi Lithium Battery for Raspberry Pi-Zero W)</t>
   </si>
 </sst>
 </file>
@@ -422,124 +440,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A4:K19"/>
+  <dimension ref="A4:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7265625" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="N4" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="H7" s="3">
+        <v>29.9</v>
+      </c>
+      <c r="K7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" s="3">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="K8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="3">
+        <v>7.8</v>
+      </c>
+      <c r="K9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" s="3">
+        <v>25.8</v>
+      </c>
+      <c r="K10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="K11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="E7" s="3">
-        <v>29.9</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3">
-        <v>36.200000000000003</v>
-      </c>
-      <c r="H8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9" s="3">
-        <v>7.8</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="H12" s="4">
+        <v>2.23</v>
+      </c>
+      <c r="K12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="4">
+        <v>27.9</v>
+      </c>
+      <c r="K13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="4">
+        <v>29.99</v>
+      </c>
+      <c r="K14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="H16" s="4"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.35">
+      <c r="C19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="3">
-        <v>25.8</v>
-      </c>
-      <c r="H10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.8</v>
-      </c>
-      <c r="H11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4">
-        <v>2.23</v>
-      </c>
-      <c r="H12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="4">
-        <v>27.9</v>
-      </c>
-      <c r="H13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E14" s="4"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="E16" s="4"/>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
-      <c r="C19" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="3">
-        <f>SUM(E7:E16)</f>
-        <v>130.63</v>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="H19" s="3">
+        <f>SUM(H7:H16)</f>
+        <v>160.62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>